<commit_message>
Added condition if any style is not here in the style guide then it will not show in mismtach and also show not found in expected
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Style Guide.xlsx
+++ b/cypress/fixtures/Style Guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raj.khajanchi\Desktop\Cypress Font size\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{636C4C6C-D770-4C25-AC3D-78E491FCACBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195AC4E8-824E-4B8C-8E8C-D70313BF32E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="I2" sqref="I2:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -597,9 +597,7 @@
       <c r="H2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="5">
-        <v>400</v>
-      </c>
+      <c r="I2" s="5"/>
       <c r="J2" s="8">
         <v>1.3</v>
       </c>
@@ -632,9 +630,7 @@
       <c r="H3" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="5">
-        <v>500</v>
-      </c>
+      <c r="I3" s="5"/>
       <c r="J3" s="8">
         <v>1.3</v>
       </c>
@@ -667,9 +663,7 @@
       <c r="H4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="5">
-        <v>400</v>
-      </c>
+      <c r="I4" s="5"/>
       <c r="J4" s="8">
         <v>1.3</v>
       </c>
@@ -702,9 +696,7 @@
       <c r="H5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="5">
-        <v>400</v>
-      </c>
+      <c r="I5" s="5"/>
       <c r="J5" s="8">
         <v>1.2</v>
       </c>
@@ -737,9 +729,7 @@
       <c r="H6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="5">
-        <v>500</v>
-      </c>
+      <c r="I6" s="5"/>
       <c r="J6" s="8">
         <v>1.1000000000000001</v>
       </c>
@@ -772,9 +762,7 @@
       <c r="H7" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I7" s="5">
-        <v>500</v>
-      </c>
+      <c r="I7" s="5"/>
       <c r="J7" s="8">
         <v>1.4</v>
       </c>
@@ -807,9 +795,7 @@
       <c r="H8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="5">
-        <v>500</v>
-      </c>
+      <c r="I8" s="5"/>
       <c r="J8" s="8">
         <v>1.4</v>
       </c>
@@ -842,9 +828,7 @@
       <c r="H9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="I9" s="5">
-        <v>500</v>
-      </c>
+      <c r="I9" s="5"/>
       <c r="J9" s="8">
         <v>1.4</v>
       </c>
@@ -877,9 +861,7 @@
       <c r="H10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="5">
-        <v>500</v>
-      </c>
+      <c r="I10" s="5"/>
       <c r="J10" s="8">
         <v>1.4</v>
       </c>
@@ -912,9 +894,7 @@
       <c r="H11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="5">
-        <v>500</v>
-      </c>
+      <c r="I11" s="5"/>
       <c r="J11" s="8">
         <v>1.4</v>
       </c>
@@ -947,9 +927,7 @@
       <c r="H12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="5">
-        <v>400</v>
-      </c>
+      <c r="I12" s="5"/>
       <c r="J12" s="8">
         <v>1.4</v>
       </c>
@@ -982,9 +960,7 @@
       <c r="H13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="5">
-        <v>400</v>
-      </c>
+      <c r="I13" s="5"/>
       <c r="J13" s="8">
         <v>1.4</v>
       </c>

</xml_diff>

<commit_message>
URLs json has been updated for the multiple URLs can fetch and per page putfile will be generated
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Style Guide.xlsx
+++ b/cypress/fixtures/Style Guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raj.khajanchi\Desktop\Cypress Font size\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195AC4E8-824E-4B8C-8E8C-D70313BF32E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48605626-1DBE-486A-912C-287D1366BB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -519,7 +519,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Maded the read of the headers
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Style Guide.xlsx
+++ b/cypress/fixtures/Style Guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raj.khajanchi\Desktop\Cypress Font size\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48605626-1DBE-486A-912C-287D1366BB2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F483BCFD-674E-477C-A1BA-A3503025C244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="35">
   <si>
     <t>H1</t>
   </si>
@@ -516,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6531BB6-DDF6-4ED1-83DC-D125CF295C5E}">
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -529,15 +529,14 @@
     <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
     <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" style="1" customWidth="1"/>
     <col min="7" max="7" width="11.140625" customWidth="1"/>
     <col min="8" max="9" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" customWidth="1"/>
     <col min="12" max="12" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" s="3" t="s">
         <v>20</v>
       </c>
@@ -553,8 +552,8 @@
       <c r="E1" s="3">
         <v>1201</v>
       </c>
-      <c r="F1" s="3">
-        <v>991</v>
+      <c r="F1" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="G1" s="3">
         <v>767</v>
@@ -568,11 +567,8 @@
       <c r="J1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
@@ -588,8 +584,8 @@
       <c r="E2" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="8" t="s">
-        <v>23</v>
+      <c r="F2" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G2" s="8" t="s">
         <v>23</v>
@@ -601,11 +597,8 @@
       <c r="J2" s="8">
         <v>1.3</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="13" t="s">
         <v>3</v>
       </c>
@@ -621,8 +614,8 @@
       <c r="E3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>25</v>
+      <c r="F3" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>25</v>
@@ -634,11 +627,8 @@
       <c r="J3" s="8">
         <v>1.3</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="13" t="s">
         <v>3</v>
       </c>
@@ -654,8 +644,8 @@
       <c r="E4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>25</v>
+      <c r="F4" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G4" s="8" t="s">
         <v>25</v>
@@ -667,11 +657,8 @@
       <c r="J4" s="8">
         <v>1.3</v>
       </c>
-      <c r="K4" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="13" t="s">
         <v>3</v>
       </c>
@@ -687,8 +674,8 @@
       <c r="E5" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>10</v>
+      <c r="F5" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>10</v>
@@ -700,11 +687,8 @@
       <c r="J5" s="8">
         <v>1.2</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6" s="13" t="s">
         <v>3</v>
       </c>
@@ -720,8 +704,8 @@
       <c r="E6" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>10</v>
+      <c r="F6" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G6" s="8" t="s">
         <v>10</v>
@@ -733,11 +717,8 @@
       <c r="J6" s="8">
         <v>1.1000000000000001</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7" s="13" t="s">
         <v>3</v>
       </c>
@@ -753,8 +734,8 @@
       <c r="E7" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>11</v>
+      <c r="F7" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G7" s="8" t="s">
         <v>11</v>
@@ -766,11 +747,8 @@
       <c r="J7" s="8">
         <v>1.4</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="13" t="s">
         <v>4</v>
       </c>
@@ -786,8 +764,8 @@
       <c r="E8" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>12</v>
+      <c r="F8" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G8" s="8" t="s">
         <v>12</v>
@@ -799,11 +777,8 @@
       <c r="J8" s="8">
         <v>1.4</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="13" t="s">
         <v>5</v>
       </c>
@@ -819,8 +794,8 @@
       <c r="E9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>1</v>
+      <c r="F9" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>1</v>
@@ -832,11 +807,8 @@
       <c r="J9" s="8">
         <v>1.4</v>
       </c>
-      <c r="K9" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="13" t="s">
         <v>6</v>
       </c>
@@ -852,8 +824,8 @@
       <c r="E10" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>13</v>
+      <c r="F10" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>13</v>
@@ -865,11 +837,8 @@
       <c r="J10" s="8">
         <v>1.4</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="13" t="s">
         <v>7</v>
       </c>
@@ -885,8 +854,8 @@
       <c r="E11" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>14</v>
+      <c r="F11" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>14</v>
@@ -898,11 +867,8 @@
       <c r="J11" s="8">
         <v>1.4</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="13" t="s">
         <v>28</v>
       </c>
@@ -918,8 +884,8 @@
       <c r="E12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>8</v>
+      <c r="F12" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G12" s="8" t="s">
         <v>8</v>
@@ -931,11 +897,8 @@
       <c r="J12" s="8">
         <v>1.4</v>
       </c>
-      <c r="K12" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" s="13" t="s">
         <v>29</v>
       </c>
@@ -951,8 +914,8 @@
       <c r="E13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>9</v>
+      <c r="F13" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>9</v>
@@ -964,22 +927,18 @@
       <c r="J13" s="8">
         <v>1.4</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14" s="5"/>
       <c r="B14" s="6"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
-      <c r="K14" s="5"/>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="2"/>

</xml_diff>

<commit_message>
Now the div eleemts will be come in the output fuile and code is also optimized
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Style Guide.xlsx
+++ b/cypress/fixtures/Style Guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raj.khajanchi\Desktop\Cypress Font size\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F483BCFD-674E-477C-A1BA-A3503025C244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF1A221-F2E7-42F3-A11F-D13FEDF8D8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="36">
   <si>
     <t>H1</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>190px</t>
+  </si>
+  <si>
+    <t>div</t>
   </si>
 </sst>
 </file>
@@ -519,7 +522,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -929,16 +932,36 @@
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="A14" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="2"/>

</xml_diff>

<commit_message>
Still need to check and align the labels proeprly
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Style Guide.xlsx
+++ b/cypress/fixtures/Style Guide.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raj.khajanchi\Desktop\Cypress Font size\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{765C4C58-A84D-4E7A-B509-C90A917D0EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F9F9187-3762-4A98-A33E-AF9646707728}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -529,7 +529,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -547,7 +547,7 @@
     <col min="12" max="12" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="28.5">
+    <row r="1" spans="1:10" ht="14.25">
       <c r="A1" s="7" t="s">
         <v>34</v>
       </c>

</xml_diff>